<commit_message>
Refactor VDP cartridge bus and address logic
Updated signal naming and bus/address decoding logic across msx_slot, ip_gpio, and vdp_cpu_interface modules. Replaced and reorganized internal signals for improved clarity and correctness, including changes to address decoding, rdata enable, and palette logic. Adjusted LUT and DFF instantiations to match new signal structure and fixed several combinatorial and sequential logic paths.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$3:$F$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$3:$F$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -301,6 +301,16 @@
   </si>
   <si>
     <t>STOP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>衝突座標</t>
+    <rPh sb="0" eb="2">
+      <t>ショウトツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ザヒョウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -688,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G49"/>
+  <dimension ref="A2:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1096,7 +1106,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -1111,10 +1121,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1129,10 +1139,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>12</v>
@@ -1153,10 +1163,10 @@
         <v>31</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
@@ -1171,16 +1181,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <v>0</v>
@@ -1195,13 +1205,13 @@
         <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="4">
         <v>0</v>
@@ -1216,10 +1226,10 @@
         <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
@@ -1234,10 +1244,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>14</v>
@@ -1258,7 +1268,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>14</v>
@@ -1279,7 +1289,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>14</v>
@@ -1300,7 +1310,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>14</v>
@@ -1321,7 +1331,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>14</v>
@@ -1342,7 +1352,7 @@
         <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>14</v>
@@ -1363,7 +1373,7 @@
         <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>14</v>
@@ -1384,7 +1394,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>14</v>
@@ -1405,7 +1415,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
@@ -1426,7 +1436,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>14</v>
@@ -1447,7 +1457,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>14</v>
@@ -1468,7 +1478,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>14</v>
@@ -1489,26 +1499,38 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="D40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
@@ -1592,9 +1614,18 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="E3:F39">
+  <conditionalFormatting sqref="E3:F40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Refactor VDP cartridge logic and signal names
Updated RTL implementation for the tangnano20k VDP cartridge, including significant refactoring of internal wire and signal names, LUT logic, and register assignments. These changes improve code clarity, maintainability, and align with new palette and register handling requirements.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$3:$F$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$3:$F$41</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -311,6 +311,14 @@
     <rPh sb="2" eb="4">
       <t>ザヒョウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パレット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カラーパレット</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -698,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G50"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -992,19 +1000,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -1016,13 +1024,13 @@
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E16" s="4">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -1037,16 +1045,16 @@
         <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -1058,16 +1066,16 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2"/>
     </row>
@@ -1079,7 +1087,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>14</v>
@@ -1100,13 +1108,13 @@
         <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -1121,10 +1129,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1142,13 +1150,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -1160,16 +1168,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -1184,10 +1192,10 @@
         <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
@@ -1202,10 +1210,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>14</v>
@@ -1226,13 +1234,13 @@
         <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4">
         <v>0</v>
@@ -1247,10 +1255,10 @@
         <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -1265,10 +1273,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>14</v>
@@ -1289,7 +1297,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>14</v>
@@ -1310,7 +1318,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>14</v>
@@ -1331,7 +1339,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>14</v>
@@ -1352,7 +1360,7 @@
         <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>14</v>
@@ -1373,7 +1381,7 @@
         <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>14</v>
@@ -1394,7 +1402,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>14</v>
@@ -1415,7 +1423,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
@@ -1436,7 +1444,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>14</v>
@@ -1457,7 +1465,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>14</v>
@@ -1478,7 +1486,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>14</v>
@@ -1499,7 +1507,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>14</v>
@@ -1520,26 +1528,38 @@
         <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0</v>
-      </c>
-      <c r="F40" s="4">
-        <v>0</v>
-      </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="D41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -1623,9 +1643,18 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="E3:F40">
+  <conditionalFormatting sqref="E3:F41">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Update VDP logic and timing control modules
Refactors and expands the VDP timing control logic, including changes to LUT definitions, signal wiring, and module interfaces. Updates include new and renamed outputs, adjustments to combinational logic, and improved handling of horizontal and vertical timing signals. These changes likely address timing, feature expansion, or bug fixes in the video display processor implementation.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -319,6 +319,69 @@
   </si>
   <si>
     <t>カラーパレット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CPU I/F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VRAM書き込み</t>
+    <rPh sb="4" eb="5">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VRAM読みだし</t>
+    <rPh sb="4" eb="5">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コントロールレジスタ書き込み</t>
+    <rPh sb="10" eb="11">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>間接コントロールレジスタ書き込み</t>
+    <rPh sb="0" eb="2">
+      <t>カンセツ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ステータスレジスタ読みだし</t>
+    <rPh sb="9" eb="10">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インターレースモード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>50Hz モード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SSG</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -708,15 +771,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="12.25" customWidth="1"/>
-    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.25" customWidth="1"/>
     <col min="7" max="7" width="52.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1033,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -1243,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G26" s="2"/>
     </row>
@@ -1261,10 +1324,10 @@
         <v>15</v>
       </c>
       <c r="E27" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G27" s="2"/>
     </row>
@@ -1282,10 +1345,10 @@
         <v>14</v>
       </c>
       <c r="E28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1563,66 +1626,150 @@
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="4">
+        <v>1</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.3</v>
+      </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.3</v>
+      </c>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
@@ -1655,6 +1802,114 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E3:F41">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42:F42">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43:F43">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:F44">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45:F45">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:F48">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Refactor and update VDP timing and LED control logic
Reworked LUT and wire assignments in tangnano20k_vdp_cartridge.vg, including significant changes to VDP timing control, LED logic, and signal naming. Updated module interfaces and internal connections for vdp_timing_control_ssg, changing several port names and signal groupings. These changes improve clarity, maintainability, and correctness of the synthesized design.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A2:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2"/>
     </row>
@@ -1327,7 +1327,7 @@
         <v>0.3</v>
       </c>
       <c r="F27" s="4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G27" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor WS2812 LED logic and fix signal assignments
Reworked the WS2812 LED driver logic in the synthesized netlist, including major changes to LUT assignments, signal ordering, and state machine logic. Fixed undeclared symbol warnings and improved the structure of the generated Verilog. These changes improve maintainability and correctness of the LED control logic.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A2:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor and expand VDP interface and testbenches
Major refactoring of the VDP CPU interface and MSX slot modules, including changes to port widths, signal naming, and logic for address and data handling. Updated and expanded testbenches for SCREEN0 and SCREEN1, and reorganized test_top files into SCREEN-specific directories. Adjusted synthesis and implementation files to match the new design. These changes improve modularity, support for multiple screen modes, and clarify signal usage throughout the design.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor VDP cartridge and CPU interface logic
Major update to the VDP cartridge and vdp_cpu_interface modules, including changes to input/output ports, LUT logic, and signal wiring. Removed and replaced several signals, restructured address and interrupt handling, and added new DFFCE registers. These changes improve clarity, fix wiring issues, and enhance support for additional screen modes and interrupt logic.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1324,10 +1324,10 @@
         <v>15</v>
       </c>
       <c r="E27" s="4">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="F27" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G27" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update VDP and testbench files, add new test cases
Significant updates to vdp_cpu_interface.v and related Verilog modules, including changes to signal names, logic, and interface definitions. Added new test programs (SC4TEST.COM, SC5TEST.COM, TEST.COM) and their corresponding assembly sources. Updated synthesis, implementation, and documentation files to reflect these changes. These modifications improve VDP functionality and expand test coverage.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add SCREEN8 testbench and update VDP logic
Introduces a new SCREEN8 testbench with supporting Verilog and batch files. Updates vdp.v and vdp_cpu_interface.v to refactor address and interrupt logic, add new signals, and improve handling of VRAM and status registers. Also adds new VDP software tests and updates documentation and synthesis outputs.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G11" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor VDP cartridge logic and update interfaces
Significant changes to the VDP cartridge Verilog netlist and logic, including reordering and renaming of signals, LUT and DFFCE logic updates, and interface adjustments. These changes improve signal clarity, update address and data path handling, and enhance interrupt and register logic for the VDP cartridge implementation. Associated testbenches, reports, and synthesis outputs have been updated accordingly.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1576,10 +1576,10 @@
         <v>14</v>
       </c>
       <c r="E39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -1597,10 +1597,10 @@
         <v>14</v>
       </c>
       <c r="E40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2"/>
     </row>
@@ -1618,10 +1618,10 @@
         <v>14</v>
       </c>
       <c r="E41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G41" s="2"/>
     </row>
@@ -1663,7 +1663,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2"/>
     </row>
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="2"/>
     </row>
@@ -1726,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G46" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update development history and progress documentation
Added entries for August 18 and 19, 2025, detailing the implementation of the VDP Command LINE, bug fixes related to BUSDIR and cache memory, and updates to ensure proper operation. Also updated the progress tracking spreadsheet.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A2:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1534,10 +1534,10 @@
         <v>14</v>
       </c>
       <c r="E37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G37" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor VDP status register and interrupt logic
Major changes to the VDP core and timing modules, including refactoring the status register pointer to a multi-bit bus, updating interrupt and frame/line logic, and reorganizing signal names and connections. These changes improve clarity, fix potential bugs, and enhance the flexibility of the VDP implementation. Project and synthesis settings were also updated to increase loop limits and enable more warnings.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1429,10 +1429,10 @@
         <v>14</v>
       </c>
       <c r="E32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G32" s="2"/>
     </row>
@@ -1513,10 +1513,10 @@
         <v>14</v>
       </c>
       <c r="E36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G36" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor and update VDP interface and synthesis outputs
Significant changes were made to the VDP (Video Display Processor) interface, including renaming and restructuring of internal signals, LUTs, and module ports. The synthesis and PNR output files were updated to reflect these changes. New test and documentation files were added for the soft VDP test, and related batch and log files were updated. These changes improve clarity, maintainability, and expand test coverage for the VDP cartridge project.
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A2:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1369,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G29" s="2"/>
     </row>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G33" s="2"/>
     </row>
@@ -1471,7 +1471,7 @@
         <v>14</v>
       </c>
       <c r="E34" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F34" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Sprite mode1 bug fixed
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="2"/>
     </row>
@@ -1330,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Added VRAM 256KB mode
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1246,7 +1246,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -1939,7 +1939,7 @@
         <v>64</v>
       </c>
       <c r="E52" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Extended Color Palette Mode Implementation Complete
32768色中256色モードを実装した。
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1960,10 +1960,10 @@
         <v>64</v>
       </c>
       <c r="E53" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F53" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2"/>
     </row>

</xml_diff>

<commit_message>
Bugfix Sprite outside on upper
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1218,10 +1218,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added R#20 bit1 (SVNS)
</commit_message>
<xml_diff>
--- a/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
+++ b/RTL/tangnano20k_vdp_cartridge_step7/src/th9958/doc/th9958_progress.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1911,10 +1911,10 @@
         <v>64</v>
       </c>
       <c r="E50" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="2"/>
     </row>
@@ -2040,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G56" s="2"/>
     </row>

</xml_diff>